<commit_message>
smtp pool feature added
</commit_message>
<xml_diff>
--- a/spread_sheets/student_data.xlsx
+++ b/spread_sheets/student_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -31,22 +31,28 @@
     <t>subject</t>
   </si>
   <si>
+    <t>body</t>
+  </si>
+  <si>
     <t>Lakshman</t>
   </si>
   <si>
     <t>manojathi.14@gmail.com</t>
   </si>
   <si>
-    <t>completed</t>
+    <t>not completed</t>
+  </si>
+  <si>
+    <t>task incomplete</t>
+  </si>
+  <si>
+    <t>Lorem ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
   </si>
   <si>
     <t>Ram</t>
   </si>
   <si>
     <t>Seetha</t>
-  </si>
-  <si>
-    <t>not completed</t>
   </si>
   <si>
     <t>Hanuman</t>
@@ -77,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -89,13 +95,24 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -112,6 +129,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -349,26 +369,32 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <f>DATE(2022, 5, 23)</f>
         <v>44704</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -376,20 +402,23 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <f>DATE(2022, 5, 24)</f>
         <v>44705</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -397,20 +426,23 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
         <f>DATE(2022, 5, 22)</f>
         <v>44703</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -418,20 +450,23 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C11" si="1">DATE(2022, 5, 25)</f>
+        <f t="shared" ref="C5:C24" si="1">DATE(2022, 5, 25)</f>
         <v>44706</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -439,20 +474,23 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -460,20 +498,23 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -481,20 +522,23 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -502,20 +546,23 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -523,20 +570,23 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -544,24 +594,336 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
         <v>44706</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="2"/>
+      <c r="A12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="1"/>
+        <v>44706</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>